<commit_message>
Changes without switch case
</commit_message>
<xml_diff>
--- a/testData/testdata.xlsx
+++ b/testData/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18483\eclipse-workspace\SeleniumTestNGJava\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18483\eclipse-workspace\SeleniumTestNGJava01\TestNG-Maven-Selenium\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32D3AD2-4BBD-49B7-9D20-29506AC634CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73987FA-BBC6-49B0-AC4B-B94FED1D0B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{3B8E28A9-4F3F-42DF-900D-069796F94DBC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3B8E28A9-4F3F-42DF-900D-069796F94DBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Search Text</t>
   </si>
@@ -55,7 +55,13 @@
     <t>https://google.com</t>
   </si>
   <si>
-    <t>mytestdata1</t>
+    <t>https://www.bing.com/</t>
+  </si>
+  <si>
+    <t>Text3</t>
+  </si>
+  <si>
+    <t>Text4</t>
   </si>
 </sst>
 </file>
@@ -407,15 +413,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE9EC04-CB33-442E-8756-2DCCF9E08CF5}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -450,14 +457,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>6</v>
+      <c r="B6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>